<commit_message>
Cập nhật 2 cột QCStatus và QCNote khi xuât dữ liệu ra file export. Chỉnh sửa truy xuất dữ liệu đếm số lần viếng thăm.
</commit_message>
<xml_diff>
--- a/SourceCode/EmployeeTracking.Admin/ExcelTemplate/ReportTemplate.xlsx
+++ b/SourceCode/EmployeeTracking.Admin/ExcelTemplate/ReportTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hung\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOLPHINS\EmployeeTracking\SourceCode\EmployeeTracking.Admin\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Báo cáo" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
   <si>
     <t>Ngày thực hiện</t>
   </si>
@@ -178,12 +178,18 @@
   </si>
   <si>
     <t>Thành công</t>
+  </si>
+  <si>
+    <t>Trạng thái QC</t>
+  </si>
+  <si>
+    <t>QC Note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -251,6 +257,11 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -260,11 +271,6 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,448 +551,465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AP4"/>
+  <dimension ref="A2:AR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AQ4" sqref="AQ4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" style="4" customWidth="1"/>
-    <col min="17" max="17" width="16" style="4" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.28515625" style="4" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" style="4" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" style="4" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" style="4" customWidth="1"/>
-    <col min="28" max="28" width="15" style="4" customWidth="1"/>
-    <col min="29" max="29" width="17.28515625" style="4" customWidth="1"/>
-    <col min="30" max="30" width="16.42578125" style="4" customWidth="1"/>
-    <col min="31" max="31" width="16.140625" style="4" customWidth="1"/>
-    <col min="32" max="32" width="15.85546875" style="4" customWidth="1"/>
-    <col min="33" max="33" width="16.28515625" style="4" customWidth="1"/>
-    <col min="34" max="34" width="18.140625" style="4" customWidth="1"/>
-    <col min="35" max="35" width="13.85546875" style="4" customWidth="1"/>
-    <col min="36" max="36" width="14" style="4" customWidth="1"/>
-    <col min="37" max="37" width="12.85546875" style="4" customWidth="1"/>
-    <col min="38" max="38" width="25.140625" style="4" customWidth="1"/>
-    <col min="39" max="39" width="22.28515625" style="4" customWidth="1"/>
-    <col min="40" max="40" width="24.7109375" style="4" customWidth="1"/>
-    <col min="41" max="41" width="14.5703125" style="4" customWidth="1"/>
-    <col min="42" max="42" width="21" style="4" customWidth="1"/>
-    <col min="43" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.88671875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="13.88671875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="14.109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="15" style="1" customWidth="1"/>
+    <col min="29" max="29" width="17.33203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="16.44140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="16.109375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15.88671875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="16.33203125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="18.109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="13.88671875" style="1" customWidth="1"/>
+    <col min="36" max="36" width="14" style="1" customWidth="1"/>
+    <col min="37" max="37" width="12.88671875" style="1" customWidth="1"/>
+    <col min="38" max="38" width="25.109375" style="1" customWidth="1"/>
+    <col min="39" max="39" width="22.33203125" style="1" customWidth="1"/>
+    <col min="40" max="40" width="24.6640625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="14.5546875" style="1" customWidth="1"/>
+    <col min="42" max="42" width="21" style="1" customWidth="1"/>
+    <col min="43" max="44" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:42">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:44">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AC2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AD2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AE2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AI2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AK2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AL2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AM2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AN2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AO2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AP2" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="AQ2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" spans="1:42">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:44">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AB3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AC3" s="5" t="s">
+      <c r="AC3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AD3" s="5" t="s">
+      <c r="AD3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AE3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AF3" s="5" t="s">
+      <c r="AF3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AG3" s="5" t="s">
+      <c r="AG3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AH3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AI3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AK3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AL3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AM3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AN3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AO3" s="1" t="s">
+      <c r="AO3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AP3" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="AQ3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:42">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:44">
+      <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y4" s="6">
+      <c r="P4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y4" s="3">
         <v>0</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="Z4" s="3">
         <v>0</v>
       </c>
-      <c r="AA4" s="6">
+      <c r="AA4" s="3">
         <v>0</v>
       </c>
-      <c r="AB4" s="6">
+      <c r="AB4" s="3">
         <v>0</v>
       </c>
-      <c r="AC4" s="6">
+      <c r="AC4" s="3">
         <v>0</v>
       </c>
-      <c r="AD4" s="6">
+      <c r="AD4" s="3">
         <v>0</v>
       </c>
-      <c r="AE4" s="6">
+      <c r="AE4" s="3">
         <v>0</v>
       </c>
-      <c r="AF4" s="6">
+      <c r="AF4" s="3">
         <v>0</v>
       </c>
-      <c r="AG4" s="6">
+      <c r="AG4" s="3">
         <v>0</v>
       </c>
-      <c r="AH4" s="6">
+      <c r="AH4" s="3">
         <v>27</v>
       </c>
-      <c r="AI4" s="6">
+      <c r="AI4" s="3">
         <v>4</v>
       </c>
-      <c r="AJ4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM4" s="6" t="s">
+      <c r="AJ4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AN4" s="6" t="s">
+      <c r="AN4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AO4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP4" s="6" t="s">
+      <c r="AO4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
+  <mergeCells count="20">
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="AH2:AH3"/>
     <mergeCell ref="AI2:AI3"/>
@@ -995,11 +1018,11 @@
     <mergeCell ref="G2:O2"/>
     <mergeCell ref="P2:X2"/>
     <mergeCell ref="Y2:AG2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>